<commit_message>
Deleted old "total" executions.
</commit_message>
<xml_diff>
--- a/results/classification/iris/executions_results_total.xlsx
+++ b/results/classification/iris/executions_results_total.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>architecture</t>
   </si>
@@ -92,70 +92,64 @@
     <t>20</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>nnnn/nnnnn/nnn</t>
   </si>
   <si>
     <t>nnnn/nnnn/nnn</t>
   </si>
   <si>
+    <t>nnnn/nnnnnn/nnn</t>
+  </si>
+  <si>
     <t>nnnn/nnn/nnn</t>
   </si>
   <si>
-    <t>nnnn/nnnnnn/nnn</t>
+    <t>nnnn/nnnnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnnnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnnnn/nnnnnn/nnn</t>
   </si>
   <si>
     <t>nnnn/nnnnn/nnnnn/nnn</t>
   </si>
   <si>
-    <t>nnnn/nnnnnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nn/nnn</t>
+    <t>nnnn/nnnnnnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnnnnnn/nnnnnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnnnnnnnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnn/n/nnnn/nnnn/n/nnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnnnnn/nnnnnnn/nnnnnnn/nnnnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnn/nnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnnn/n/nnnnn/nnnnn/n/nnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnn/nnnn/nnnnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnn/nnnn/nnnn/nnn</t>
+  </si>
+  <si>
+    <t>nnnn/nnnnnn/nnnnnn/nnnnn/nnn</t>
   </si>
   <si>
     <t>nnnn/nnnnnnnnnn/nnn</t>
   </si>
   <si>
-    <t>nnnn/nnnnnnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnnn/nnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnn/nnn/nnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnnnnnn/nnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nn/nn/nnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/n/nn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nn/nnnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nn/nn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnnn/nn/nn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnnnnn/nnnnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnnnnnnnnnnnn/nnnnnnnnnnnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnnn/nnnn/nnnn/nnnn/nnn</t>
-  </si>
-  <si>
-    <t>nnnn/nnnn/nnn/nnn</t>
+    <t>nnnn/nnnnnnnn/nnnnnnnn/nnnnnnnn/nnnnnnnn/nnn</t>
   </si>
 </sst>
 </file>
@@ -232,22 +226,22 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>0.987545787589454</v>
+        <v>0.9825396827604405</v>
       </c>
       <c r="D2" t="n">
-        <v>0.971794857428624</v>
+        <v>0.966666665342119</v>
       </c>
       <c r="E2" t="n">
-        <v>0.964102566242218</v>
+        <v>0.9962962965170542</v>
       </c>
       <c r="F2" t="n">
-        <v>13.854707397589323</v>
+        <v>28.567477648788028</v>
       </c>
       <c r="G2" t="n">
-        <v>16.25</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="3">
@@ -255,22 +249,22 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9926739926739927</v>
+        <v>0.9787114848275812</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9564102337910578</v>
+        <v>0.9705882352941176</v>
       </c>
       <c r="E3" t="n">
-        <v>0.964102566242218</v>
+        <v>0.9764705896377563</v>
       </c>
       <c r="F3" t="n">
-        <v>15.209659133629922</v>
+        <v>28.590975259332094</v>
       </c>
       <c r="G3" t="n">
-        <v>16.25</v>
+        <v>21.25</v>
       </c>
     </row>
     <row r="4">
@@ -278,22 +272,22 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9888888888888889</v>
+        <v>0.979831932906677</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9722221990426382</v>
+        <v>0.9627450914943919</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9722222238779068</v>
+        <v>0.9960784316062927</v>
       </c>
       <c r="F4" t="n">
-        <v>14.273035737640335</v>
+        <v>31.023406596277272</v>
       </c>
       <c r="G4" t="n">
-        <v>15.0</v>
+        <v>21.25</v>
       </c>
     </row>
     <row r="5">
@@ -301,22 +295,22 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9896103897652069</v>
+        <v>0.9752380954651605</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9696969444101508</v>
+        <v>0.9666666626930237</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9575757601044395</v>
+        <v>1.0</v>
       </c>
       <c r="F5" t="n">
-        <v>21.771828813275906</v>
+        <v>26.32787763039272</v>
       </c>
       <c r="G5" t="n">
-        <v>13.75</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="6">
@@ -324,22 +318,22 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="n">
-        <v>0.990476190570801</v>
+        <v>0.9873015876800295</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9555555383364359</v>
+        <v>0.9777777791023254</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9666666686534882</v>
+        <v>1.0</v>
       </c>
       <c r="F6" t="n">
-        <v>14.426801798376756</v>
+        <v>19.73988404675766</v>
       </c>
       <c r="G6" t="n">
-        <v>7.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="7">
@@ -347,22 +341,22 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9885714286849613</v>
+        <v>0.9873015873015873</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9733333110809326</v>
+        <v>0.9555555383364359</v>
       </c>
       <c r="E7" t="n">
-        <v>0.946666669845581</v>
+        <v>1.0</v>
       </c>
       <c r="F7" t="n">
-        <v>31.81478847294384</v>
+        <v>30.8073609113693</v>
       </c>
       <c r="G7" t="n">
-        <v>6.25</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="8">
@@ -370,22 +364,22 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9873015874908084</v>
+        <v>0.9809523812362126</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9555555383364359</v>
+        <v>0.9666666686534882</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.9666666686534882</v>
       </c>
       <c r="F8" t="n">
-        <v>5.402166473865506</v>
+        <v>26.8273805161317</v>
       </c>
       <c r="G8" t="n">
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9">
@@ -393,19 +387,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9857142859981174</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.9666666686534882</v>
       </c>
       <c r="F9" t="n">
-        <v>13.604894574483254</v>
+        <v>35.047248200575496</v>
       </c>
       <c r="G9" t="n">
         <v>2.5</v>
@@ -416,19 +410,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="n">
         <v>0.9857142857142858</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9833333194255829</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9666666686534882</v>
+        <v>1.0</v>
       </c>
       <c r="F10" t="n">
-        <v>17.6669285046723</v>
+        <v>35.1133285999298</v>
       </c>
       <c r="G10" t="n">
         <v>2.5</v>
@@ -439,22 +433,22 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="n">
         <v>0.9904761904761905</v>
       </c>
       <c r="D11" t="n">
-        <v>0.949999988079071</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9666666686534882</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="F11" t="n">
-        <v>28.299374716348137</v>
+        <v>11.2289566000303</v>
       </c>
       <c r="G11" t="n">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="12">
@@ -462,19 +456,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9904761904761905</v>
+        <v>0.9809523815200443</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9666666388511658</v>
+        <v>1.0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9333333373069763</v>
+        <v>1.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1.14253914528423</v>
+        <v>17.1249912699064</v>
       </c>
       <c r="G12" t="n">
         <v>1.25</v>
@@ -485,10 +479,10 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9904761904761905</v>
+        <v>0.9904761910438538</v>
       </c>
       <c r="D13" t="n">
         <v>1.0</v>
@@ -497,7 +491,7 @@
         <v>1.0</v>
       </c>
       <c r="F13" t="n">
-        <v>2.27955144584179</v>
+        <v>17.1510696848234</v>
       </c>
       <c r="G13" t="n">
         <v>1.25</v>
@@ -508,19 +502,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="n">
-        <v>1.0</v>
+        <v>0.9619047624724252</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9333333373069763</v>
+        <v>1.0</v>
       </c>
       <c r="E14" t="n">
         <v>1.0</v>
       </c>
       <c r="F14" t="n">
-        <v>3.05302775303523</v>
+        <v>18.4992587486903</v>
       </c>
       <c r="G14" t="n">
         <v>1.25</v>
@@ -531,19 +525,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="n">
         <v>0.9904761904761905</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="E15" t="n">
         <v>1.0</v>
       </c>
       <c r="F15" t="n">
-        <v>3.61325516700745</v>
+        <v>31.7194145321846</v>
       </c>
       <c r="G15" t="n">
         <v>1.25</v>
@@ -554,19 +548,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="n">
         <v>0.9904761904761905</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8999999761581421</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="E16" t="n">
         <v>0.9333333373069763</v>
       </c>
       <c r="F16" t="n">
-        <v>4.98083841403325</v>
+        <v>31.7597713828087</v>
       </c>
       <c r="G16" t="n">
         <v>1.25</v>
@@ -577,19 +571,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="n">
-        <v>1.0</v>
+        <v>0.9809523809523809</v>
       </c>
       <c r="D17" t="n">
         <v>0.9666666388511658</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9333333373069763</v>
+        <v>1.0</v>
       </c>
       <c r="F17" t="n">
-        <v>5.11930145025253</v>
+        <v>33.1587646325429</v>
       </c>
       <c r="G17" t="n">
         <v>1.25</v>
@@ -600,19 +594,19 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9904761904761905</v>
+        <v>0.9809523809523809</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8666666746139526</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="F18" t="n">
-        <v>16.5964641491572</v>
+        <v>36.5265705664953</v>
       </c>
       <c r="G18" t="n">
         <v>1.25</v>
@@ -623,19 +617,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9904761904761905</v>
+        <v>0.9809523809523809</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9333333373069763</v>
+        <v>1.0</v>
       </c>
       <c r="F19" t="n">
-        <v>23.6605709671974</v>
+        <v>36.966023349762</v>
       </c>
       <c r="G19" t="n">
         <v>1.25</v>
@@ -646,7 +640,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" t="n">
         <v>0.9904761904761905</v>
@@ -655,10 +649,10 @@
         <v>0.9333333373069763</v>
       </c>
       <c r="E20" t="n">
-        <v>1.0</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="F20" t="n">
-        <v>25.435343849659</v>
+        <v>37.7258544484774</v>
       </c>
       <c r="G20" t="n">
         <v>1.25</v>
@@ -669,44 +663,21 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9904761904761905</v>
+        <v>0.9809523809523809</v>
       </c>
       <c r="D21" t="n">
         <v>1.0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9333333373069763</v>
+        <v>1.0</v>
       </c>
       <c r="F21" t="n">
-        <v>34.777114033699</v>
+        <v>37.9731294512749</v>
       </c>
       <c r="G21" t="n">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.9904761904761905</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.9666666388511658</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>58.3761653145154</v>
-      </c>
-      <c r="G22" t="n">
         <v>1.25</v>
       </c>
     </row>

</xml_diff>